<commit_message>
change UI: remove unecessary stuff
</commit_message>
<xml_diff>
--- a/Document/Khảo sát câu hỏi (960 câu).xlsx
+++ b/Document/Khảo sát câu hỏi (960 câu).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/1512413_student_hcmus_edu_vn/Documents/Đề tài khóa luận Chatbot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\Study\Chatbot-Thesis\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{DBBEC32B-847C-4687-A6AD-E274F98BB1AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4DD85487-313E-4932-961A-A97744368BFF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6812B5CB-152D-4B61-BA80-EEA51DC65C2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{94F733B5-282F-D442-A322-265BEFC355FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94F733B5-282F-D442-A322-265BEFC355FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2624,7 +2624,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -2667,7 +2667,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2965,19 +2965,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D6E179-AB95-D641-AE08-AADC2C2C4F94}">
   <dimension ref="A1:H396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="1" max="1" width="42.625" customWidth="1"/>
     <col min="2" max="2" width="58.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="50.625" customWidth="1"/>
     <col min="4" max="4" width="21.125" customWidth="1"/>
     <col min="5" max="5" width="58.125" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="6" max="6" width="239.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>